<commit_message>
worked on fake stuff
</commit_message>
<xml_diff>
--- a/Peter/StuffyStuff/assets/data/CBH_AnnualReport-ComptesConsolides_2016/CBH_AnnualReport-ComptesConsolides_2016.xlsx
+++ b/Peter/StuffyStuff/assets/data/CBH_AnnualReport-ComptesConsolides_2016/CBH_AnnualReport-ComptesConsolides_2016.xlsx
@@ -6275,7 +6275,7 @@
       <selection activeCell="G9" sqref="G9:G14"/>
       <selection pane="topRight" activeCell="G9" sqref="G9:G14"/>
       <selection pane="bottomLeft" activeCell="G9" sqref="G9:G14"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0"/>
@@ -6328,10 +6328,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="24">
-        <v>220734331</v>
+        <v>987654321</v>
       </c>
       <c r="C3" s="25">
-        <v>164230739</v>
+        <v>123456789</v>
       </c>
       <c r="G3" s="67"/>
       <c r="H3" s="67"/>
@@ -6517,11 +6517,11 @@
       </c>
       <c r="B14" s="26">
         <f>SUM(B3:B13)</f>
-        <v>2433876656</v>
+        <v>3200796646</v>
       </c>
       <c r="C14" s="27">
         <f>SUM(C3:C13)</f>
-        <v>2277059060</v>
+        <v>2236285110</v>
       </c>
       <c r="G14" s="69">
         <f>SUM(G3:G13)</f>
@@ -6927,11 +6927,11 @@
     <row r="39" spans="1:9" ht="19" customHeight="1">
       <c r="B39" s="7">
         <f>+B14-B34</f>
-        <v>0</v>
+        <v>766919990</v>
       </c>
       <c r="C39" s="7">
         <f>+C14-C34</f>
-        <v>0</v>
+        <v>-40773950</v>
       </c>
       <c r="G39" s="67"/>
       <c r="H39" s="67"/>
@@ -10721,7 +10721,7 @@
       </c>
       <c r="J5" s="28">
         <f>ROUND((+C_Bilan!B3/1000),0)-H5</f>
-        <v>0</v>
+        <v>766920</v>
       </c>
       <c r="L5" s="67"/>
       <c r="M5" s="67"/>
@@ -10955,7 +10955,7 @@
       </c>
       <c r="J12" s="116">
         <f>ROUND(SUM(C_Bilan!B3:B8)/1000,0)-H12</f>
-        <v>1</v>
+        <v>766920</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="24" customHeight="1">
@@ -10989,7 +10989,7 @@
       </c>
       <c r="J13" s="28">
         <f>ROUND(SUM(C_Bilan!C3:C8)/1000,0)-H13</f>
-        <v>-1</v>
+        <v>-40775</v>
       </c>
       <c r="L13" s="67">
         <f>+L8+L9</f>
@@ -11320,11 +11320,11 @@
       </c>
       <c r="F4" s="119">
         <f>ROUND(+C_Bilan!B3/1000,0)-SUM(B4:C4)</f>
-        <v>0</v>
+        <v>766920</v>
       </c>
       <c r="G4" s="119">
         <f>ROUND(+C_Bilan!C3/1000,0)-SUM(D4:E4)</f>
-        <v>0</v>
+        <v>-40774</v>
       </c>
       <c r="I4" s="67"/>
       <c r="J4" s="67"/>
@@ -11678,11 +11678,11 @@
       </c>
       <c r="F15" s="120">
         <f>ROUND(+C_Bilan!B14/1000,0)-SUM(B15:C15)</f>
-        <v>0</v>
+        <v>766920</v>
       </c>
       <c r="G15" s="120">
         <f>ROUND(+C_Bilan!C14/1000,0)-SUM(D15:E15)</f>
-        <v>-1</v>
+        <v>-40775</v>
       </c>
       <c r="I15" s="69">
         <f>SUM(I4:I14)</f>
@@ -12462,7 +12462,7 @@
       </c>
       <c r="G10" s="10">
         <f>+B10-C_Bilan!B14/1000</f>
-        <v>0.34400000004097819</v>
+        <v>-766919.64600000018</v>
       </c>
     </row>
   </sheetData>
@@ -12945,7 +12945,7 @@
       </c>
       <c r="J3" s="28">
         <f>ROUND((+C_Bilan!B3/1000),0)-G3</f>
-        <v>0</v>
+        <v>766920</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="24" customHeight="1">
@@ -13293,7 +13293,7 @@
       </c>
       <c r="J14" s="28">
         <f>ROUND((+C_Bilan!B14/1000),0)-G14</f>
-        <v>0</v>
+        <v>766920</v>
       </c>
       <c r="L14" s="69">
         <f>SUM(L3:L13)</f>

</xml_diff>